<commit_message>
fix: Rerun the RNAseq metadata reharmonization procedure
</commit_message>
<xml_diff>
--- a/metadata/rnaseq/todo/California Institute of Technology TMC (RNAseq).xlsx
+++ b/metadata/rnaseq/todo/California Institute of Technology TMC (RNAseq).xlsx
@@ -13,6 +13,7 @@
     <sheet name="Invalid Input Pattern" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Standard Value'!$A$1:$E$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Missing Required Value'!$A$1:$D$109</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Invalid Input Pattern'!$A$1:$F$13</definedName>
   </definedNames>
@@ -419,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,404 +429,467 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>ng/ul</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>ul</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 8 rxns; PN 1000370</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>10x Genomics; Chromium i7 Multiplex Kit, 96 rxns; PN 120262</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>hour</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2" t="n">
+        <v>16</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>pg/ul</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>ng</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Next GEM Automated Single Cell 5' Kit v2, 4 rxns; PN 1000298</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Illumina; TruSeq RNA CD Index Plate (96 Indexes, 96 Samples); PN 20019792</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>month</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3" t="n">
+        <v>40</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>nM</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 4 slides, 16 reactions; PN 1000184</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Not applicable</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>year</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="C4" t="inlineStr">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1,27</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>8,8,8</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Parse Biosciences; Evercode WT v2 Kit, 48 rxns; PN ECW02030</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Illumina; TruSeq RNA Single Indexes Set A (12 Indexes, 48 Samples); PN 20020492</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>day</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="C5" t="inlineStr">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0,38,76</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>8,6</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 16 rxns; PN 1000263</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Illumina; TruSeq RNA Single Indexes Set B (12 Indexes, 48 Samples); PN 20020493</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>minute</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="C6" t="inlineStr">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10,48,78</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Human Transcriptome, 1 slides, 4 reactions; PN 1000338</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium i7 Sample Index Plate (96 rxn); PN 220103</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="C7" t="inlineStr">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>10,48,86</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 16 rxns; PN 1000268</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-AB</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="C8" t="inlineStr">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0,20-23,41-44</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>10x Genomics; Chromium Next GEM Single Cell ATAC Library &amp; Gel Bead Kit, 16 rxns; PN 1000175</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-CD</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="C9" t="inlineStr">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>10x Genomics; Library Construction Kit C, 16 rxns; PN 1000694</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-EF</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="C10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>10x Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Mouse Transcriptome, 6.5mm, 4 rxns; PN 1000521</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>NanoString Technologies; GeoMx Seq Code Pack; PN GMX-NGS-SEQ-GH</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="C11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Next GEM Single Cell 3' HT Kit v3.1, 48 rxns; PN 1000348</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Custom</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="C12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Next GEM Single Cell 3' GEM, Library &amp; Gel Bead Kit v3.1, 16 rxns; PN 1000121</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>10x Genomics; Chromium i7 Multiplex Kit N, Set A, 96 rxn; PN 1000084</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="C13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>10x Genomics; Library Construction Kit C, 4 rxns; PN 1000689</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>Parse Biosciences; Fragmentation Reagents; PN WX100</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="C14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 11 mm, 2 reactions; PN 1000522</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>Integrated DNA Technologies: Custom DNA Oligos</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="C15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>Illumina; TruSeq Stranded mRNA Library Prep (48 samples); PN 20020594</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>Parse Biosciences; UDI Plate - WT; PN UDI1001</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="C16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>10X Genomics; Automated Library Construction Kit, 24 rxns; PN 1000428</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>10X Genomics; Dual Index Kit TS, Set A; PN 1000251</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="C17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>New England BioLabs; NEBNext Ultra II RNA Library Prep Kit for Illumina; PN E7770</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>Illumina; IDT for Illumina - TruSeq RNA UD Indexes v2 (96 Indexes, 96 Samples); PN 20040871</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="C18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Next GEM Automated Single Cell 5' Kit v2, 24 rxns; PN 1000290</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>10X Genomics; Single Index Kit N, Set A (96 rxn); PN 1000212</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="C19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 1 slides, 4 reactions; PN 1000187</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>10X Genomics; Dual Index Kit TT, Set A (96 rxn); PN 1000215</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="C20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>10x Genomics; Chromium GEM-X Single Cell 5' Kit v3, 16 rxns; PN 1000699</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="C21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>10x Genomics; Chromium Single Cell ATAC Library &amp; Gel Bead Kit, 16 rxns; PN 1000110</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="C22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>10x Genomics; Library Construction Kit, 16 rxns; PN 1000190</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="C23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>Parse Biosciences; Evercode WT Mini v2 Kit, 12 rxns; PN ECW02010</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="C24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>10x Genomics; Chromium Next GEM Single Cell 5' HT Kit v2, 48 rxns; PN 1000356</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="C25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>Illumina; TruSeq Stranded mRNA Library Prep (96 samples); PN 20020595</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="C26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Next GEM Single Cell 5' Kit v2, 4 rxns; PN 1000265</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="C27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 4 rxn; PN 1000285</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="C28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Hybridization &amp; Library Kit, 4 rxns; PN 1000415</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="C29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>Custom</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="C30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Single Cell 3' GEM, Library &amp; Gel Bead Kit v3, 4 rxns; PN 1000092</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="C31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>10x Genomics; Chromium Single Cell 3ʹ GEM, Library &amp; Gel Bead Kit v3, 16 rxns; PN 1000075</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="C32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Single Cell 3' Library &amp; Gel Bead Kit, 4 rxns; PN 120267</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="C33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Mouse Transcriptome, 4 rxns; PN 1000339</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="C34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 16 rxn; PN 1000283</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="C35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>10X Genomics; Chromium Next GEM Single Cell 3' Kit v3.1, 4 rxns; PN 1000269</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="C36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>10x Genomics; Chromium Next GEM Single Cell 5' HT Kit v2, 8 rxns; PN 1000374</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="C37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 6.5mm, 4 reactions; PN 1000520</t>
         </is>
@@ -842,7 +906,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -877,7 +941,568 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>HBM258.BWHR.287</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM258.BWHR.287</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>HBM258.BWHR.287</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM258.BWHR.287</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>HBM388.ZSNN.945</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM388.ZSNN.945</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HBM388.ZSNN.945</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM388.ZSNN.945</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>HBM625.PTSS.252</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM625.PTSS.252</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HBM625.PTSS.252</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM625.PTSS.252</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>HBM645.XLLN.924</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM645.XLLN.924</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HBM645.XLLN.924</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM645.XLLN.924</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>HBM667.ZCQC.777</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM667.ZCQC.777</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>HBM667.ZCQC.777</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM667.ZCQC.777</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HBM725.RHWH.487</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM725.RHWH.487</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>HBM725.RHWH.487</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM725.RHWH.487</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>HBM737.WSXM.893</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM737.WSXM.893</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>HBM737.WSXM.893</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM737.WSXM.893</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>HBM788.XLZL.369</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM788.XLZL.369</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>HBM788.XLZL.369</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM788.XLZL.369</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>HBM849.TWBF.722</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM849.TWBF.722</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>HBM849.TWBF.722</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM849.TWBF.722</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>HBM865.KZMC.828</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM865.KZMC.828</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>HBM865.KZMC.828</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM865.KZMC.828</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>HBM965.GWBH.574</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM965.GWBH.574</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>HBM965.GWBH.574</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM965.GWBH.574</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>HBM972.VRNF.956</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>barcode_offset</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0,14</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM972.VRNF.956</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>HBM972.VRNF.956</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>barcode_size</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>10,10</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://portal.hubmapconsortium.org/browse/HBM972.VRNF.956</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:E25"/>
+  <dataValidations count="2">
+    <dataValidation sqref="D2 D4 D6 D8 D10 D12 D14 D16 D18 D20 D22 D24" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
+      <formula1>_validation_data!$A$1:$A$9</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3 D5 D7 D9 D11 D13 D15 D17 D19 D21 D23 D25" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
+      <formula1>_validation_data!$B$1:$B$6</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2866,19 +3491,19 @@
   <autoFilter ref="A1:D109"/>
   <dataValidations count="5">
     <dataValidation sqref="C2 C11 C20 C29 C38 C47 C56 C65 C74 C83 C92 C101" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$A$1:$A$3</formula1>
+      <formula1>_validation_data!$C$1:$C$3</formula1>
     </dataValidation>
     <dataValidation sqref="C4 C13 C22 C31 C40 C49 C58 C67 C76 C85 C94 C103" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$B$1:$B$2</formula1>
+      <formula1>_validation_data!$D$1:$D$2</formula1>
     </dataValidation>
     <dataValidation sqref="C6 C15 C24 C33 C42 C51 C60 C69 C78 C87 C96 C105" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$C$1:$C$37</formula1>
+      <formula1>_validation_data!$E$1:$E$37</formula1>
     </dataValidation>
     <dataValidation sqref="C7 C16 C25 C34 C43 C52 C61 C70 C79 C88 C97 C106" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$D$1:$D$19</formula1>
+      <formula1>_validation_data!$F$1:$F$19</formula1>
     </dataValidation>
     <dataValidation sqref="C9 C18 C27 C36 C45 C54 C63 C72 C81 C90 C99 C108" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$E$1:$E$5</formula1>
+      <formula1>_validation_data!$G$1:$G$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>